<commit_message>
some docstrings and basic typechecking
</commit_message>
<xml_diff>
--- a/data_NFL2025.xlsx
+++ b/data_NFL2025.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="200">
   <si>
     <t>Team1</t>
   </si>
@@ -173,52 +173,52 @@
     <t>Chicago Bears</t>
   </si>
   <si>
-    <t>1,Thu,2025-09-04,8:20PM,Philadelphia Eagles,,Dallas Cowboys,boxscore,24,20,302,0,307,1</t>
-  </si>
-  <si>
-    <t>1,Fri,2025-09-05,8:00PM,Los Angeles Chargers,,Kansas City Chiefs,boxscore,27,21,394,0,347,0</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,1:00PM,Tampa Bay Buccaneers,@,Atlanta Falcons,boxscore,23,20,260,0,358,0</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,1:00PM,Jacksonville Jaguars,,Carolina Panthers,boxscore,26,10,378,1,255,3</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,1:00PM,Cincinnati Bengals,@,Cleveland Browns,boxscore,17,16,141,0,327,2</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,1:00PM,Indianapolis Colts,,Miami Dolphins,boxscore,33,8,418,0,211,3</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,1:00PM,Arizona Cardinals,@,New Orleans Saints,boxscore,20,13,276,0,315,0</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,1:00PM,Las Vegas Raiders,@,New England Patriots,boxscore,20,13,389,1,336,1</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,1:00PM,Washington Commanders,,New York Giants,boxscore,21,6,432,0,231,0</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,1:00PM,Pittsburgh Steelers,@,New York Jets,boxscore,34,32,271,0,394,1</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,4:05PM,Denver Broncos,,Tennessee Titans,boxscore,20,12,317,4,133,2</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,4:05PM,San Francisco 49ers,@,Seattle Seahawks,boxscore,17,13,384,2,230,2</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,4:25PM,Green Bay Packers,,Detroit Lions,boxscore,27,13,266,0,246,1</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,4:25PM,Los Angeles Rams,,Houston Texans,boxscore,14,9,296,1,265,2</t>
-  </si>
-  <si>
-    <t>1,Sun,2025-09-07,8:20PM,Buffalo Bills,,Baltimore Ravens,boxscore,41,40,497,0,432,1</t>
-  </si>
-  <si>
-    <t>1,Mon,2025-09-08,8:15PM,Minnesota Vikings,@,Chicago Bears,boxscore,27,24,254,1,317,1</t>
+    <t>4,Thu,2025-09-25,8:15PM,Seattle Seahawks,@,Arizona Cardinals,boxscore,23,20,384,1,253,2</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,9:30AM,Pittsburgh Steelers,,Minnesota Vikings,boxscore,24,21,313,0,372,2</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,1:00PM,Detroit Lions,,Cleveland Browns,boxscore,34,10,277,1,249,3</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,1:00PM,Buffalo Bills,,New Orleans Saints,boxscore,31,19,356,1,298,1</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,1:00PM,Atlanta Falcons,,Washington Commanders,boxscore,34,27,435,1,294,1</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,1:00PM,New York Giants,,Los Angeles Chargers,boxscore,21,18,250,0,338,2</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,1:00PM,New England Patriots,,Carolina Panthers,boxscore,42,13,307,0,326,0</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,1:00PM,Houston Texans,,Tennessee Titans,boxscore,26,0,353,0,175,1</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,1:00PM,Philadelphia Eagles,@,Tampa Bay Buccaneers,boxscore,31,25,200,0,376,2</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,4:05PM,Jacksonville Jaguars,@,San Francisco 49ers,boxscore,26,21,325,0,389,4</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,4:05PM,Los Angeles Rams,,Indianapolis Colts,boxscore,27,20,462,1,333,3</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,4:25PM,Chicago Bears,@,Las Vegas Raiders,boxscore,25,24,271,1,357,4</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,4:25PM,Kansas City Chiefs,,Baltimore Ravens,boxscore,37,20,382,0,360,2</t>
+  </si>
+  <si>
+    <t>4,Sun,2025-09-28,8:20PM,Green Bay Packers,@,Dallas Cowboys,boxscore,40,40,489,1,436,0</t>
+  </si>
+  <si>
+    <t>4,Mon,2025-09-29,7:15PM,New York Jets,@,Miami Dolphins,preview,,,,,,</t>
+  </si>
+  <si>
+    <t>4,Mon,2025-09-29,8:15PM,Cincinnati Bengals,@,Denver Broncos,preview,,,,,,</t>
   </si>
   <si>
     <t>Full Name</t>
@@ -1403,816 +1403,1200 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="4">
+        <v>27.0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="4">
+        <v>18.0</v>
+      </c>
       <c r="E18" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Green Bay Packers</v>
       </c>
       <c r="F18" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
+      <c r="A19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="4">
+        <v>31.0</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4">
+        <v>17.0</v>
+      </c>
       <c r="E19" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Seattle Seahawks</v>
       </c>
       <c r="F19" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
+      <c r="A20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="4">
+        <v>33.0</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="4">
+        <v>19.0</v>
+      </c>
       <c r="E20" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Los Angeles Rams</v>
       </c>
       <c r="F20" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
+      <c r="A21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="4">
+        <v>10.0</v>
+      </c>
       <c r="E21" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Buffalo Bills</v>
       </c>
       <c r="F21" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
+      <c r="A22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="4">
+        <v>26.0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="4">
+        <v>21.0</v>
+      </c>
       <c r="E22" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>San Francisco 49ers</v>
       </c>
       <c r="F22" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
+      <c r="A23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4">
+        <v>33.0</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="4">
+        <v>27.0</v>
+      </c>
       <c r="E23" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>New England Patriots</v>
       </c>
       <c r="F23" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
+      <c r="A24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="4">
+        <v>52.0</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="4">
+        <v>21.0</v>
+      </c>
       <c r="E24" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Detroit Lions</v>
       </c>
       <c r="F24" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
+      <c r="A25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="4">
+        <v>40.0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="4">
+        <v>37.0</v>
+      </c>
       <c r="E25" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Dallas Cowboys</v>
       </c>
       <c r="F25" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
+      <c r="A26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="4">
+        <v>31.0</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="4">
+        <v>27.0</v>
+      </c>
       <c r="E26" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Cincinnati Bengals</v>
       </c>
       <c r="F26" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
+      <c r="A27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="4">
+        <v>41.0</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="4">
+        <v>17.0</v>
+      </c>
       <c r="E27" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Baltimore Ravens</v>
       </c>
       <c r="F27" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
+      <c r="A28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="4">
+        <v>29.0</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="4">
+        <v>28.0</v>
+      </c>
       <c r="E28" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Indianapolis Colts</v>
       </c>
       <c r="F28" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="6"/>
+      <c r="A29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="4">
+        <v>27.0</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="4">
+        <v>22.0</v>
+      </c>
       <c r="E29" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Arizona Cardinals</v>
       </c>
       <c r="F29" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
+      <c r="A30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="4">
+        <v>17.0</v>
+      </c>
       <c r="E30" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Philadelphia Eagles</v>
       </c>
       <c r="F30" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="6"/>
+      <c r="A31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="4">
+        <v>22.0</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="4">
+        <v>6.0</v>
+      </c>
       <c r="E31" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Atlanta Falcons</v>
       </c>
       <c r="F31" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
+      <c r="A32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="4">
+        <v>19.0</v>
+      </c>
       <c r="E32" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Tampa Bay Buccaneers</v>
       </c>
       <c r="F32" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6"/>
+      <c r="A33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="4">
+        <v>9.0</v>
+      </c>
       <c r="E33" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Los Angeles Chargers</v>
       </c>
       <c r="F33" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="6"/>
+      <c r="A34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="4">
+        <v>31.0</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="4">
+        <v>21.0</v>
+      </c>
       <c r="E34" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Buffalo Bills</v>
       </c>
       <c r="F34" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="6"/>
+      <c r="A35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0.0</v>
+      </c>
       <c r="E35" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Carolina Panthers</v>
       </c>
       <c r="F35" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="6"/>
+      <c r="A36" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="4">
+        <v>17.0</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="4">
+        <v>10.0</v>
+      </c>
       <c r="E36" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Jacksonville Jaguars</v>
       </c>
       <c r="F36" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="6"/>
+      <c r="A37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="4">
+        <v>41.0</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="4">
+        <v>24.0</v>
+      </c>
       <c r="E37" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Washington Commanders</v>
       </c>
       <c r="F37" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="6"/>
+      <c r="A38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="4">
+        <v>33.0</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="4">
+        <v>26.0</v>
+      </c>
       <c r="E38" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Philadelphia Eagles</v>
       </c>
       <c r="F38" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="6"/>
+      <c r="A39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="4">
+        <v>29.0</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="4">
+        <v>27.0</v>
+      </c>
       <c r="E39" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Tampa Bay Buccaneers</v>
       </c>
       <c r="F39" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="6"/>
+      <c r="A40" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="4">
+        <v>48.0</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="4">
+        <v>10.0</v>
+      </c>
       <c r="E40" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Minnesota Vikings</v>
       </c>
       <c r="F40" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="6"/>
+      <c r="A41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="4">
+        <v>13.0</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="4">
+        <v>10.0</v>
+      </c>
       <c r="E41" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Cleveland Browns</v>
       </c>
       <c r="F41" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6"/>
+      <c r="A42" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="4">
+        <v>14.0</v>
+      </c>
       <c r="E42" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Pittsburgh Steelers</v>
       </c>
       <c r="F42" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="5"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="6"/>
+      <c r="A43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="4">
+        <v>41.0</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="4">
+        <v>20.0</v>
+      </c>
       <c r="E43" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Indianapolis Colts</v>
       </c>
       <c r="F43" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
+      <c r="A44" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="4">
+        <v>44.0</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="4">
+        <v>13.0</v>
+      </c>
       <c r="E44" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Seattle Seahawks</v>
       </c>
       <c r="F44" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="5"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="6"/>
+      <c r="A45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="4">
+        <v>23.0</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="4">
+        <v>20.0</v>
+      </c>
       <c r="E45" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Los Angeles Chargers</v>
       </c>
       <c r="F45" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="6"/>
+      <c r="A46" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="4">
+        <v>31.0</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="4">
+        <v>14.0</v>
+      </c>
       <c r="E46" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Chicago Bears</v>
       </c>
       <c r="F46" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="6"/>
+      <c r="A47" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="4">
+        <v>16.0</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="4">
+        <v>15.0</v>
+      </c>
       <c r="E47" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>San Francisco 49ers</v>
       </c>
       <c r="F47" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="5"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6"/>
+      <c r="A48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="4">
+        <v>22.0</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="4">
+        <v>9.0</v>
+      </c>
       <c r="E48" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Kansas City Chiefs</v>
       </c>
       <c r="F48" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="5"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="6"/>
+      <c r="A49" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" s="4">
+        <v>38.0</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49" s="4">
+        <v>30.0</v>
+      </c>
       <c r="E49" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Detroit Lions</v>
       </c>
       <c r="F49" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="5"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="6"/>
+      <c r="A50" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="4">
+        <v>23.0</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="4">
+        <v>20.0</v>
+      </c>
       <c r="E50" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Seattle Seahawks</v>
       </c>
       <c r="F50" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="5"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="6"/>
+      <c r="A51" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="4">
+        <v>24.0</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51" s="4">
+        <v>21.0</v>
+      </c>
       <c r="E51" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Pittsburgh Steelers</v>
       </c>
       <c r="F51" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="5"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="6"/>
+      <c r="A52" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="4">
+        <v>34.0</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="4">
+        <v>10.0</v>
+      </c>
       <c r="E52" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Detroit Lions</v>
       </c>
       <c r="F52" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="5"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="6"/>
+      <c r="A53" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="4">
+        <v>31.0</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="4">
+        <v>19.0</v>
+      </c>
       <c r="E53" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Buffalo Bills</v>
       </c>
       <c r="F53" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="5"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6"/>
+      <c r="A54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="4">
+        <v>34.0</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="4">
+        <v>27.0</v>
+      </c>
       <c r="E54" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Atlanta Falcons</v>
       </c>
       <c r="F54" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="5"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="6"/>
+      <c r="A55" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="4">
+        <v>18.0</v>
+      </c>
       <c r="E55" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>New York Giants</v>
       </c>
       <c r="F55" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="5"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="6"/>
+      <c r="A56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" s="4">
+        <v>42.0</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="4">
+        <v>13.0</v>
+      </c>
       <c r="E56" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>New England Patriots</v>
       </c>
       <c r="F56" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="5"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="6"/>
+      <c r="A57" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B57" s="4">
+        <v>26.0</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" s="4">
+        <v>0.0</v>
+      </c>
       <c r="E57" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Houston Texans</v>
       </c>
       <c r="F57" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="5"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="6"/>
+      <c r="A58" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="4">
+        <v>31.0</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="4">
+        <v>25.0</v>
+      </c>
       <c r="E58" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Philadelphia Eagles</v>
       </c>
       <c r="F58" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="5"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="6"/>
+      <c r="A59" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="4">
+        <v>26.0</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" s="4">
+        <v>21.0</v>
+      </c>
       <c r="E59" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Jacksonville Jaguars</v>
       </c>
       <c r="F59" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="5"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="6"/>
+      <c r="A60" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" s="4">
+        <v>27.0</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="4">
+        <v>20.0</v>
+      </c>
       <c r="E60" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Los Angeles Rams</v>
       </c>
       <c r="F60" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="5"/>
-      <c r="B61" s="6"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="6"/>
+      <c r="A61" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" s="4">
+        <v>24.0</v>
+      </c>
       <c r="E61" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Chicago Bears</v>
       </c>
       <c r="F61" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="5"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="6"/>
+      <c r="A62" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" s="4">
+        <v>37.0</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D62" s="4">
+        <v>20.0</v>
+      </c>
       <c r="E62" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Kansas City Chiefs</v>
       </c>
       <c r="F62" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="5"/>
-      <c r="B63" s="6"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="6"/>
+      <c r="A63" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" s="4">
+        <v>40.0</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="4">
+        <v>40.0</v>
+      </c>
       <c r="E63" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>TIE</v>
       </c>
       <c r="F63" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="5"/>
-      <c r="B64" s="6"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="6"/>
+      <c r="A64" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="6">
+        <v>21.0</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="6">
+        <v>27.0</v>
+      </c>
       <c r="E64" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Miami Dolphins</v>
       </c>
       <c r="F64" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="5"/>
-      <c r="B65" s="6"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="6"/>
+      <c r="A65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" s="6">
+        <v>28.0</v>
+      </c>
       <c r="E65" s="5" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Denver Broncos</v>
       </c>
       <c r="F65" s="6" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G65" s="6" t="b">
         <v>0</v>
@@ -6319,57 +6703,60 @@
         <v>39</v>
       </c>
       <c r="B1" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A1,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A1,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C1" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Thu")</f>
         <v>Thu</v>
       </c>
       <c r="D1" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45904.0)</f>
-        <v>45904</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45925.0)</f>
+        <v>45925</v>
       </c>
       <c r="E1" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.8472222222222222)</f>
-        <v>0.8472222222</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.84375)</f>
+        <v>0.84375</v>
       </c>
       <c r="F1" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Philadelphia Eagles")</f>
-        <v>Philadelphia Eagles</v>
-      </c>
-      <c r="G1" s="8"/>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Seattle Seahawks")</f>
+        <v>Seattle Seahawks</v>
+      </c>
+      <c r="G1" s="8" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"@")</f>
+        <v>@</v>
+      </c>
       <c r="H1" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Dallas Cowboys")</f>
-        <v>Dallas Cowboys</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Arizona Cardinals")</f>
+        <v>Arizona Cardinals</v>
       </c>
       <c r="I1" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J1" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),24.0)</f>
-        <v>24</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),23.0)</f>
+        <v>23</v>
       </c>
       <c r="K1" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),20.0)</f>
         <v>20</v>
       </c>
       <c r="L1" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),302.0)</f>
-        <v>302</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),384.0)</f>
+        <v>384</v>
       </c>
       <c r="M1" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="N1" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),307.0)</f>
-        <v>307</v>
-      </c>
-      <c r="O1" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
         <v>1</v>
+      </c>
+      <c r="N1" s="8">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),253.0)</f>
+        <v>253</v>
+      </c>
+      <c r="O1" s="8">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
@@ -6377,57 +6764,57 @@
         <v>40</v>
       </c>
       <c r="B2" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A2,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A2,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C2" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Fri")</f>
-        <v>Fri</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
+        <v>Sun</v>
       </c>
       <c r="D2" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45905.0)</f>
-        <v>45905</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E2" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.8333333333333334)</f>
-        <v>0.8333333333</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3958333333333333)</f>
+        <v>0.3958333333</v>
       </c>
       <c r="F2" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Los Angeles Chargers")</f>
-        <v>Los Angeles Chargers</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Pittsburgh Steelers")</f>
+        <v>Pittsburgh Steelers</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Kansas City Chiefs")</f>
-        <v>Kansas City Chiefs</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Minnesota Vikings")</f>
+        <v>Minnesota Vikings</v>
       </c>
       <c r="I2" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J2" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),27.0)</f>
-        <v>27</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),24.0)</f>
+        <v>24</v>
       </c>
       <c r="K2" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),21.0)</f>
         <v>21</v>
       </c>
       <c r="L2" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),394.0)</f>
-        <v>394</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),313.0)</f>
+        <v>313</v>
       </c>
       <c r="M2" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
         <v>0</v>
       </c>
       <c r="N2" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),347.0)</f>
-        <v>347</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),372.0)</f>
+        <v>372</v>
       </c>
       <c r="O2" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -6435,60 +6822,57 @@
         <v>41</v>
       </c>
       <c r="B3" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A3,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A3,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C3" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
         <v>Sun</v>
       </c>
       <c r="D3" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E3" s="10">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.5416666666666666)</f>
         <v>0.5416666667</v>
       </c>
       <c r="F3" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Tampa Bay Buccaneers")</f>
-        <v>Tampa Bay Buccaneers</v>
-      </c>
-      <c r="G3" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"@")</f>
-        <v>@</v>
-      </c>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Detroit Lions")</f>
+        <v>Detroit Lions</v>
+      </c>
+      <c r="G3" s="8"/>
       <c r="H3" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Atlanta Falcons")</f>
-        <v>Atlanta Falcons</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Cleveland Browns")</f>
+        <v>Cleveland Browns</v>
       </c>
       <c r="I3" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J3" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),23.0)</f>
-        <v>23</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),34.0)</f>
+        <v>34</v>
       </c>
       <c r="K3" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),20.0)</f>
-        <v>20</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10.0)</f>
+        <v>10</v>
       </c>
       <c r="L3" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),260.0)</f>
-        <v>260</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),277.0)</f>
+        <v>277</v>
       </c>
       <c r="M3" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
       </c>
       <c r="N3" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),358.0)</f>
-        <v>358</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),249.0)</f>
+        <v>249</v>
       </c>
       <c r="O3" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -6496,57 +6880,57 @@
         <v>42</v>
       </c>
       <c r="B4" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A4,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A4,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C4" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
         <v>Sun</v>
       </c>
       <c r="D4" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E4" s="10">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.5416666666666666)</f>
         <v>0.5416666667</v>
       </c>
       <c r="F4" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Jacksonville Jaguars")</f>
-        <v>Jacksonville Jaguars</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Buffalo Bills")</f>
+        <v>Buffalo Bills</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Carolina Panthers")</f>
-        <v>Carolina Panthers</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"New Orleans Saints")</f>
+        <v>New Orleans Saints</v>
       </c>
       <c r="I4" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J4" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),26.0)</f>
-        <v>26</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),31.0)</f>
+        <v>31</v>
       </c>
       <c r="K4" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),10.0)</f>
-        <v>10</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),19.0)</f>
+        <v>19</v>
       </c>
       <c r="L4" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),378.0)</f>
-        <v>378</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),356.0)</f>
+        <v>356</v>
       </c>
       <c r="M4" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
         <v>1</v>
       </c>
       <c r="N4" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),255.0)</f>
-        <v>255</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),298.0)</f>
+        <v>298</v>
       </c>
       <c r="O4" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
-        <v>3</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -6554,60 +6938,57 @@
         <v>43</v>
       </c>
       <c r="B5" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A5,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A5,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C5" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
         <v>Sun</v>
       </c>
       <c r="D5" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E5" s="10">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.5416666666666666)</f>
         <v>0.5416666667</v>
       </c>
       <c r="F5" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Cincinnati Bengals")</f>
-        <v>Cincinnati Bengals</v>
-      </c>
-      <c r="G5" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"@")</f>
-        <v>@</v>
-      </c>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Atlanta Falcons")</f>
+        <v>Atlanta Falcons</v>
+      </c>
+      <c r="G5" s="8"/>
       <c r="H5" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Cleveland Browns")</f>
-        <v>Cleveland Browns</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Washington Commanders")</f>
+        <v>Washington Commanders</v>
       </c>
       <c r="I5" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J5" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),17.0)</f>
-        <v>17</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),34.0)</f>
+        <v>34</v>
       </c>
       <c r="K5" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),16.0)</f>
-        <v>16</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),27.0)</f>
+        <v>27</v>
       </c>
       <c r="L5" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),141.0)</f>
-        <v>141</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),435.0)</f>
+        <v>435</v>
       </c>
       <c r="M5" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
       </c>
       <c r="N5" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),327.0)</f>
-        <v>327</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),294.0)</f>
+        <v>294</v>
       </c>
       <c r="O5" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -6615,57 +6996,57 @@
         <v>44</v>
       </c>
       <c r="B6" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A6,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A6,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C6" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
         <v>Sun</v>
       </c>
       <c r="D6" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E6" s="10">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.5416666666666666)</f>
         <v>0.5416666667</v>
       </c>
       <c r="F6" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Indianapolis Colts")</f>
-        <v>Indianapolis Colts</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"New York Giants")</f>
+        <v>New York Giants</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Miami Dolphins")</f>
-        <v>Miami Dolphins</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Los Angeles Chargers")</f>
+        <v>Los Angeles Chargers</v>
       </c>
       <c r="I6" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J6" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),33.0)</f>
-        <v>33</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),21.0)</f>
+        <v>21</v>
       </c>
       <c r="K6" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),8.0)</f>
-        <v>8</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),18.0)</f>
+        <v>18</v>
       </c>
       <c r="L6" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),418.0)</f>
-        <v>418</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),250.0)</f>
+        <v>250</v>
       </c>
       <c r="M6" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
         <v>0</v>
       </c>
       <c r="N6" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),211.0)</f>
-        <v>211</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),338.0)</f>
+        <v>338</v>
       </c>
       <c r="O6" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
-        <v>3</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -6673,56 +7054,53 @@
         <v>45</v>
       </c>
       <c r="B7" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A7,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A7,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C7" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
         <v>Sun</v>
       </c>
       <c r="D7" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E7" s="10">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.5416666666666666)</f>
         <v>0.5416666667</v>
       </c>
       <c r="F7" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Arizona Cardinals")</f>
-        <v>Arizona Cardinals</v>
-      </c>
-      <c r="G7" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"@")</f>
-        <v>@</v>
-      </c>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"New England Patriots")</f>
+        <v>New England Patriots</v>
+      </c>
+      <c r="G7" s="8"/>
       <c r="H7" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"New Orleans Saints")</f>
-        <v>New Orleans Saints</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Carolina Panthers")</f>
+        <v>Carolina Panthers</v>
       </c>
       <c r="I7" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J7" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),20.0)</f>
-        <v>20</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),42.0)</f>
+        <v>42</v>
       </c>
       <c r="K7" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13.0)</f>
         <v>13</v>
       </c>
       <c r="L7" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),276.0)</f>
-        <v>276</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),307.0)</f>
+        <v>307</v>
       </c>
       <c r="M7" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
         <v>0</v>
       </c>
       <c r="N7" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),315.0)</f>
-        <v>315</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),326.0)</f>
+        <v>326</v>
       </c>
       <c r="O7" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
@@ -6734,56 +7112,53 @@
         <v>46</v>
       </c>
       <c r="B8" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A8,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A8,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C8" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
         <v>Sun</v>
       </c>
       <c r="D8" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E8" s="10">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.5416666666666666)</f>
         <v>0.5416666667</v>
       </c>
       <c r="F8" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Las Vegas Raiders")</f>
-        <v>Las Vegas Raiders</v>
-      </c>
-      <c r="G8" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"@")</f>
-        <v>@</v>
-      </c>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Houston Texans")</f>
+        <v>Houston Texans</v>
+      </c>
+      <c r="G8" s="8"/>
       <c r="H8" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"New England Patriots")</f>
-        <v>New England Patriots</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Tennessee Titans")</f>
+        <v>Tennessee Titans</v>
       </c>
       <c r="I8" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J8" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),20.0)</f>
-        <v>20</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),26.0)</f>
+        <v>26</v>
       </c>
       <c r="K8" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13.0)</f>
-        <v>13</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
+        <v>0</v>
       </c>
       <c r="L8" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),389.0)</f>
-        <v>389</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),353.0)</f>
+        <v>353</v>
       </c>
       <c r="M8" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
+        <v>0</v>
       </c>
       <c r="N8" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),336.0)</f>
-        <v>336</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),175.0)</f>
+        <v>175</v>
       </c>
       <c r="O8" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
@@ -6795,57 +7170,60 @@
         <v>47</v>
       </c>
       <c r="B9" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A9,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A9,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C9" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
         <v>Sun</v>
       </c>
       <c r="D9" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E9" s="10">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.5416666666666666)</f>
         <v>0.5416666667</v>
       </c>
       <c r="F9" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Washington Commanders")</f>
-        <v>Washington Commanders</v>
-      </c>
-      <c r="G9" s="8"/>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Philadelphia Eagles")</f>
+        <v>Philadelphia Eagles</v>
+      </c>
+      <c r="G9" s="8" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"@")</f>
+        <v>@</v>
+      </c>
       <c r="H9" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"New York Giants")</f>
-        <v>New York Giants</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Tampa Bay Buccaneers")</f>
+        <v>Tampa Bay Buccaneers</v>
       </c>
       <c r="I9" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J9" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),21.0)</f>
-        <v>21</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),31.0)</f>
+        <v>31</v>
       </c>
       <c r="K9" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),6.0)</f>
-        <v>6</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),25.0)</f>
+        <v>25</v>
       </c>
       <c r="L9" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),432.0)</f>
-        <v>432</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),200.0)</f>
+        <v>200</v>
       </c>
       <c r="M9" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
         <v>0</v>
       </c>
       <c r="N9" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),231.0)</f>
-        <v>231</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),376.0)</f>
+        <v>376</v>
       </c>
       <c r="O9" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -6853,60 +7231,60 @@
         <v>48</v>
       </c>
       <c r="B10" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A10,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A10,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C10" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
         <v>Sun</v>
       </c>
       <c r="D10" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E10" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.5416666666666666)</f>
-        <v>0.5416666667</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.6701388888888888)</f>
+        <v>0.6701388889</v>
       </c>
       <c r="F10" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Pittsburgh Steelers")</f>
-        <v>Pittsburgh Steelers</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Jacksonville Jaguars")</f>
+        <v>Jacksonville Jaguars</v>
       </c>
       <c r="G10" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"@")</f>
         <v>@</v>
       </c>
       <c r="H10" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"New York Jets")</f>
-        <v>New York Jets</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"San Francisco 49ers")</f>
+        <v>San Francisco 49ers</v>
       </c>
       <c r="I10" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J10" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),34.0)</f>
-        <v>34</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),26.0)</f>
+        <v>26</v>
       </c>
       <c r="K10" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),32.0)</f>
-        <v>32</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),21.0)</f>
+        <v>21</v>
       </c>
       <c r="L10" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),271.0)</f>
-        <v>271</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),325.0)</f>
+        <v>325</v>
       </c>
       <c r="M10" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
         <v>0</v>
       </c>
       <c r="N10" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),394.0)</f>
-        <v>394</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),389.0)</f>
+        <v>389</v>
       </c>
       <c r="O10" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.0)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -6914,57 +7292,57 @@
         <v>49</v>
       </c>
       <c r="B11" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A11,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A11,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C11" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
         <v>Sun</v>
       </c>
       <c r="D11" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E11" s="10">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.6701388888888888)</f>
         <v>0.6701388889</v>
       </c>
       <c r="F11" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Denver Broncos")</f>
-        <v>Denver Broncos</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Los Angeles Rams")</f>
+        <v>Los Angeles Rams</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Tennessee Titans")</f>
-        <v>Tennessee Titans</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Indianapolis Colts")</f>
+        <v>Indianapolis Colts</v>
       </c>
       <c r="I11" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J11" s="8">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),27.0)</f>
+        <v>27</v>
+      </c>
+      <c r="K11" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),20.0)</f>
         <v>20</v>
       </c>
-      <c r="K11" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),12.0)</f>
-        <v>12</v>
-      </c>
       <c r="L11" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),317.0)</f>
-        <v>317</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),462.0)</f>
+        <v>462</v>
       </c>
       <c r="M11" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.0)</f>
-        <v>4</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
       </c>
       <c r="N11" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),133.0)</f>
-        <v>133</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),333.0)</f>
+        <v>333</v>
       </c>
       <c r="O11" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.0)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -6972,60 +7350,60 @@
         <v>50</v>
       </c>
       <c r="B12" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A12,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A12,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C12" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
         <v>Sun</v>
       </c>
       <c r="D12" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E12" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.6701388888888888)</f>
-        <v>0.6701388889</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.6840277777777778)</f>
+        <v>0.6840277778</v>
       </c>
       <c r="F12" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"San Francisco 49ers")</f>
-        <v>San Francisco 49ers</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Chicago Bears")</f>
+        <v>Chicago Bears</v>
       </c>
       <c r="G12" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"@")</f>
         <v>@</v>
       </c>
       <c r="H12" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Seattle Seahawks")</f>
-        <v>Seattle Seahawks</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Las Vegas Raiders")</f>
+        <v>Las Vegas Raiders</v>
       </c>
       <c r="I12" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J12" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),17.0)</f>
-        <v>17</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),25.0)</f>
+        <v>25</v>
       </c>
       <c r="K12" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13.0)</f>
-        <v>13</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),24.0)</f>
+        <v>24</v>
       </c>
       <c r="L12" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),384.0)</f>
-        <v>384</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),271.0)</f>
+        <v>271</v>
       </c>
       <c r="M12" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
+        <v>1</v>
       </c>
       <c r="N12" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),230.0)</f>
-        <v>230</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),357.0)</f>
+        <v>357</v>
       </c>
       <c r="O12" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.0)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -7033,57 +7411,57 @@
         <v>51</v>
       </c>
       <c r="B13" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A13,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A13,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C13" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
         <v>Sun</v>
       </c>
       <c r="D13" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E13" s="10">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.6840277777777778)</f>
         <v>0.6840277778</v>
       </c>
       <c r="F13" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Green Bay Packers")</f>
-        <v>Green Bay Packers</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Kansas City Chiefs")</f>
+        <v>Kansas City Chiefs</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Detroit Lions")</f>
-        <v>Detroit Lions</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Baltimore Ravens")</f>
+        <v>Baltimore Ravens</v>
       </c>
       <c r="I13" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J13" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),27.0)</f>
-        <v>27</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),37.0)</f>
+        <v>37</v>
       </c>
       <c r="K13" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13.0)</f>
-        <v>13</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),20.0)</f>
+        <v>20</v>
       </c>
       <c r="L13" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),266.0)</f>
-        <v>266</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),382.0)</f>
+        <v>382</v>
       </c>
       <c r="M13" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
         <v>0</v>
       </c>
       <c r="N13" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),246.0)</f>
-        <v>246</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),360.0)</f>
+        <v>360</v>
       </c>
       <c r="O13" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -7091,57 +7469,60 @@
         <v>52</v>
       </c>
       <c r="B14" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A14,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A14,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C14" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
         <v>Sun</v>
       </c>
       <c r="D14" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45928.0)</f>
+        <v>45928</v>
       </c>
       <c r="E14" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.6840277777777778)</f>
-        <v>0.6840277778</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.8472222222222222)</f>
+        <v>0.8472222222</v>
       </c>
       <c r="F14" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Los Angeles Rams")</f>
-        <v>Los Angeles Rams</v>
-      </c>
-      <c r="G14" s="8"/>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Green Bay Packers")</f>
+        <v>Green Bay Packers</v>
+      </c>
+      <c r="G14" s="8" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"@")</f>
+        <v>@</v>
+      </c>
       <c r="H14" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Houston Texans")</f>
-        <v>Houston Texans</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Dallas Cowboys")</f>
+        <v>Dallas Cowboys</v>
       </c>
       <c r="I14" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
         <v>boxscore</v>
       </c>
       <c r="J14" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),14.0)</f>
-        <v>14</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),40.0)</f>
+        <v>40</v>
       </c>
       <c r="K14" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),9.0)</f>
-        <v>9</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),40.0)</f>
+        <v>40</v>
       </c>
       <c r="L14" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),296.0)</f>
-        <v>296</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),489.0)</f>
+        <v>489</v>
       </c>
       <c r="M14" s="8">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
         <v>1</v>
       </c>
       <c r="N14" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),265.0)</f>
-        <v>265</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),436.0)</f>
+        <v>436</v>
       </c>
       <c r="O14" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0)</f>
-        <v>2</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -7149,342 +7530,373 @@
         <v>53</v>
       </c>
       <c r="B15" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A15,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A15,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C15" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sun")</f>
-        <v>Sun</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Mon")</f>
+        <v>Mon</v>
       </c>
       <c r="D15" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45907.0)</f>
-        <v>45907</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45929.0)</f>
+        <v>45929</v>
       </c>
       <c r="E15" s="10">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.8472222222222222)</f>
-        <v>0.8472222222</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.8020833333333334)</f>
+        <v>0.8020833333</v>
       </c>
       <c r="F15" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Buffalo Bills")</f>
-        <v>Buffalo Bills</v>
-      </c>
-      <c r="G15" s="8"/>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"New York Jets")</f>
+        <v>New York Jets</v>
+      </c>
+      <c r="G15" s="8" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"@")</f>
+        <v>@</v>
+      </c>
       <c r="H15" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Baltimore Ravens")</f>
-        <v>Baltimore Ravens</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Miami Dolphins")</f>
+        <v>Miami Dolphins</v>
       </c>
       <c r="I15" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
-        <v>boxscore</v>
-      </c>
-      <c r="J15" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),41.0)</f>
-        <v>41</v>
-      </c>
-      <c r="K15" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),40.0)</f>
-        <v>40</v>
-      </c>
-      <c r="L15" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),497.0)</f>
-        <v>497</v>
-      </c>
-      <c r="M15" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0)</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),432.0)</f>
-        <v>432</v>
-      </c>
-      <c r="O15" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
-      </c>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"preview")</f>
+        <v>preview</v>
+      </c>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B16" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A16,"","",,false)"),1.0)</f>
-        <v>1</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("SPLIT(A16,"","",,false)"),4.0)</f>
+        <v>4</v>
       </c>
       <c r="C16" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Mon")</f>
         <v>Mon</v>
       </c>
       <c r="D16" s="9">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45908.0)</f>
-        <v>45908</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),45929.0)</f>
+        <v>45929</v>
       </c>
       <c r="E16" s="10">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.84375)</f>
         <v>0.84375</v>
       </c>
       <c r="F16" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Minnesota Vikings")</f>
-        <v>Minnesota Vikings</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Cincinnati Bengals")</f>
+        <v>Cincinnati Bengals</v>
       </c>
       <c r="G16" s="8" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"@")</f>
         <v>@</v>
       </c>
       <c r="H16" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Chicago Bears")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Denver Broncos")</f>
+        <v>Denver Broncos</v>
+      </c>
+      <c r="I16" s="8" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"preview")</f>
+        <v>preview</v>
+      </c>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+    </row>
+    <row r="19">
+      <c r="D19" s="8" t="str">
+        <f t="shared" ref="D19:D34" si="1">F1</f>
+        <v>Seattle Seahawks</v>
+      </c>
+      <c r="E19" s="8">
+        <f t="shared" ref="E19:E34" si="2">J1</f>
+        <v>23</v>
+      </c>
+      <c r="F19" s="8" t="str">
+        <f t="shared" ref="F19:F34" si="3">H1</f>
+        <v>Arizona Cardinals</v>
+      </c>
+      <c r="G19" s="8">
+        <f t="shared" ref="G19:G34" si="4">K1</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="D20" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Pittsburgh Steelers</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="F20" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Minnesota Vikings</v>
+      </c>
+      <c r="G20" s="8">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="D21" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Detroit Lions</v>
+      </c>
+      <c r="E21" s="8">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="F21" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Cleveland Browns</v>
+      </c>
+      <c r="G21" s="8">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="D22" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Buffalo Bills</v>
+      </c>
+      <c r="E22" s="8">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="F22" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>New Orleans Saints</v>
+      </c>
+      <c r="G22" s="8">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Atlanta Falcons</v>
+      </c>
+      <c r="E23" s="8">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="F23" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Washington Commanders</v>
+      </c>
+      <c r="G23" s="8">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="D24" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>New York Giants</v>
+      </c>
+      <c r="E24" s="8">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="F24" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Los Angeles Chargers</v>
+      </c>
+      <c r="G24" s="8">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="D25" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>New England Patriots</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="F25" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Carolina Panthers</v>
+      </c>
+      <c r="G25" s="8">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="D26" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Houston Texans</v>
+      </c>
+      <c r="E26" s="8">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="F26" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Tennessee Titans</v>
+      </c>
+      <c r="G26" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="D27" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Philadelphia Eagles</v>
+      </c>
+      <c r="E27" s="8">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="F27" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Tampa Bay Buccaneers</v>
+      </c>
+      <c r="G27" s="8">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Jacksonville Jaguars</v>
+      </c>
+      <c r="E28" s="8">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="F28" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>San Francisco 49ers</v>
+      </c>
+      <c r="G28" s="8">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="D29" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Los Angeles Rams</v>
+      </c>
+      <c r="E29" s="8">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="F29" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Indianapolis Colts</v>
+      </c>
+      <c r="G29" s="8">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" s="8" t="str">
+        <f t="shared" si="1"/>
         <v>Chicago Bears</v>
       </c>
-      <c r="I16" s="8" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"boxscore")</f>
-        <v>boxscore</v>
-      </c>
-      <c r="J16" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),27.0)</f>
-        <v>27</v>
-      </c>
-      <c r="K16" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),24.0)</f>
+      <c r="E30" s="8">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="F30" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Las Vegas Raiders</v>
+      </c>
+      <c r="G30" s="8">
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="L16" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),254.0)</f>
-        <v>254</v>
-      </c>
-      <c r="M16" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
-      </c>
-      <c r="N16" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),317.0)</f>
-        <v>317</v>
-      </c>
-      <c r="O16" s="8">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="D19" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="8">
-        <v>24.0</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="8">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="D20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="8">
-        <v>27.0</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="8">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="D21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="8">
-        <v>23.0</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="8">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="D22" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="8">
-        <v>26.0</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="8">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="D23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="8">
-        <v>17.0</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="8">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="D24" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="8">
-        <v>33.0</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="8">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="D25" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="8">
-        <v>20.0</v>
-      </c>
-      <c r="F25" s="8" t="s">
+    </row>
+    <row r="31">
+      <c r="D31" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Kansas City Chiefs</v>
+      </c>
+      <c r="E31" s="8">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="F31" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Baltimore Ravens</v>
+      </c>
+      <c r="G31" s="8">
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="G25" s="8">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="D26" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="8">
-        <v>20.0</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="8">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="D27" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="8">
-        <v>21.0</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="8">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="D28" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="8">
-        <v>34.0</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28" s="8">
-        <v>32.0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="D29" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="8">
-        <v>20.0</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" s="8">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="D30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="8">
-        <v>17.0</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30" s="8">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="D31" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="8">
-        <v>27.0</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G31" s="8">
-        <v>13.0</v>
-      </c>
     </row>
     <row r="32">
-      <c r="D32" s="8" t="s">
-        <v>33</v>
+      <c r="D32" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Green Bay Packers</v>
       </c>
       <c r="E32" s="8">
-        <v>14.0</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>34</v>
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="F32" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Dallas Cowboys</v>
       </c>
       <c r="G32" s="8">
-        <v>9.0</v>
+        <f t="shared" si="4"/>
+        <v>40</v>
       </c>
     </row>
     <row r="33">
-      <c r="D33" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" s="8">
-        <v>41.0</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G33" s="8">
-        <v>40.0</v>
+      <c r="D33" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>New York Jets</v>
+      </c>
+      <c r="E33" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F33" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Miami Dolphins</v>
+      </c>
+      <c r="G33" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
     <row r="34">
-      <c r="D34" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="8">
-        <v>27.0</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G34" s="8">
-        <v>24.0</v>
+      <c r="D34" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Cincinnati Bengals</v>
+      </c>
+      <c r="E34" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F34" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v>Denver Broncos</v>
+      </c>
+      <c r="G34" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>